<commit_message>
Aggiornato con l'ultima ottimizzazione
</commit_message>
<xml_diff>
--- a/Ottimizzazioni.xlsx
+++ b/Ottimizzazioni.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="11700"/>
@@ -11,12 +11,12 @@
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="143">
   <si>
     <t>3018.22</t>
   </si>
@@ -223,13 +223,235 @@
   </si>
   <si>
     <t>GBPUSD</t>
+  </si>
+  <si>
+    <t>EURUSD</t>
+  </si>
+  <si>
+    <t>1.42</t>
+  </si>
+  <si>
+    <t>26.02</t>
+  </si>
+  <si>
+    <t>2811.99</t>
+  </si>
+  <si>
+    <t>18.31%</t>
+  </si>
+  <si>
+    <t>1.41</t>
+  </si>
+  <si>
+    <t>25.53</t>
+  </si>
+  <si>
+    <t>2801.00</t>
+  </si>
+  <si>
+    <t>18.37%</t>
+  </si>
+  <si>
+    <t>1.34</t>
+  </si>
+  <si>
+    <t>23.07</t>
+  </si>
+  <si>
+    <t>2154.58</t>
+  </si>
+  <si>
+    <t>18.24</t>
+  </si>
+  <si>
+    <t>21.59</t>
+  </si>
+  <si>
+    <t>2376.24</t>
+  </si>
+  <si>
+    <t>17.46%</t>
+  </si>
+  <si>
+    <t>19.55</t>
+  </si>
+  <si>
+    <t>3281.91</t>
+  </si>
+  <si>
+    <t>21.57%</t>
+  </si>
+  <si>
+    <t>1.33</t>
+  </si>
+  <si>
+    <t>17.35</t>
+  </si>
+  <si>
+    <t>2421.05</t>
+  </si>
+  <si>
+    <t>17.81%</t>
+  </si>
+  <si>
+    <t>15.74</t>
+  </si>
+  <si>
+    <t>3300.21</t>
+  </si>
+  <si>
+    <t>23.00%</t>
+  </si>
+  <si>
+    <t>8949.49</t>
+  </si>
+  <si>
+    <t>1.56</t>
+  </si>
+  <si>
+    <t>40.87</t>
+  </si>
+  <si>
+    <t>2189.87</t>
+  </si>
+  <si>
+    <t>19.64%</t>
+  </si>
+  <si>
+    <t>8914.05</t>
+  </si>
+  <si>
+    <t>40.70</t>
+  </si>
+  <si>
+    <t>2175.17</t>
+  </si>
+  <si>
+    <t>19.49%</t>
+  </si>
+  <si>
+    <t>7883.36</t>
+  </si>
+  <si>
+    <t>1.50</t>
+  </si>
+  <si>
+    <t>36.16</t>
+  </si>
+  <si>
+    <t>2446.64</t>
+  </si>
+  <si>
+    <t>22.80%</t>
+  </si>
+  <si>
+    <t>7411.93</t>
+  </si>
+  <si>
+    <t>34.16</t>
+  </si>
+  <si>
+    <t>2462.61</t>
+  </si>
+  <si>
+    <t>22.01%</t>
+  </si>
+  <si>
+    <t>6972.06</t>
+  </si>
+  <si>
+    <t>1.43</t>
+  </si>
+  <si>
+    <t>32.13</t>
+  </si>
+  <si>
+    <t>2781.71</t>
+  </si>
+  <si>
+    <t>25.59%</t>
+  </si>
+  <si>
+    <t>SL_added_pips=45</t>
+  </si>
+  <si>
+    <t>5272.93</t>
+  </si>
+  <si>
+    <t>24.08</t>
+  </si>
+  <si>
+    <t>3300.84</t>
+  </si>
+  <si>
+    <t>31.18%</t>
+  </si>
+  <si>
+    <t>5177.08</t>
+  </si>
+  <si>
+    <t>1.35</t>
+  </si>
+  <si>
+    <t>23.53</t>
+  </si>
+  <si>
+    <t>2903.00</t>
+  </si>
+  <si>
+    <t>29.39%</t>
+  </si>
+  <si>
+    <t>5108.32</t>
+  </si>
+  <si>
+    <t>23.33</t>
+  </si>
+  <si>
+    <t>3213.74</t>
+  </si>
+  <si>
+    <t>30.78%</t>
+  </si>
+  <si>
+    <t>4340.26</t>
+  </si>
+  <si>
+    <t>1.30</t>
+  </si>
+  <si>
+    <t>19.29</t>
+  </si>
+  <si>
+    <t>3036.15</t>
+  </si>
+  <si>
+    <t>29.48%</t>
+  </si>
+  <si>
+    <t>3971.37</t>
+  </si>
+  <si>
+    <t>17.81</t>
+  </si>
+  <si>
+    <t>3458.16</t>
+  </si>
+  <si>
+    <t>33.64%</t>
+  </si>
+  <si>
+    <t>AUDUSD</t>
+  </si>
+  <si>
+    <t>0.0000000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,8 +467,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,12 +491,16 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -268,17 +508,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Nota" xfId="2" builtinId="10"/>
+    <cellStyle name="Valore valido" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -570,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A19:W28"/>
+  <dimension ref="A8:W38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -593,44 +854,694 @@
     <col min="21" max="21" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="8" spans="1:23">
+      <c r="A8" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>213</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O9" t="s">
+        <v>12</v>
+      </c>
+      <c r="P9" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>14</v>
+      </c>
+      <c r="R9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S9" t="s">
+        <v>16</v>
+      </c>
+      <c r="T9" t="s">
+        <v>17</v>
+      </c>
+      <c r="U9" t="s">
+        <v>18</v>
+      </c>
+      <c r="V9" t="s">
+        <v>19</v>
+      </c>
+      <c r="W9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>213</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" t="s">
+        <v>10</v>
+      </c>
+      <c r="N10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" t="s">
+        <v>12</v>
+      </c>
+      <c r="P10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>14</v>
+      </c>
+      <c r="R10" t="s">
+        <v>15</v>
+      </c>
+      <c r="S10" t="s">
+        <v>16</v>
+      </c>
+      <c r="T10" t="s">
+        <v>17</v>
+      </c>
+      <c r="U10" t="s">
+        <v>18</v>
+      </c>
+      <c r="V10" t="s">
+        <v>19</v>
+      </c>
+      <c r="W10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11">
+        <v>211</v>
+      </c>
+      <c r="D11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" t="s">
+        <v>8</v>
+      </c>
+      <c r="L11" t="s">
+        <v>9</v>
+      </c>
+      <c r="M11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N11" t="s">
+        <v>11</v>
+      </c>
+      <c r="O11" t="s">
+        <v>12</v>
+      </c>
+      <c r="P11" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>14</v>
+      </c>
+      <c r="R11" t="s">
+        <v>15</v>
+      </c>
+      <c r="S11" t="s">
+        <v>16</v>
+      </c>
+      <c r="T11" t="s">
+        <v>17</v>
+      </c>
+      <c r="U11" t="s">
+        <v>18</v>
+      </c>
+      <c r="V11" t="s">
+        <v>19</v>
+      </c>
+      <c r="W11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12">
+        <v>211</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" t="s">
+        <v>8</v>
+      </c>
+      <c r="L12" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" t="s">
+        <v>10</v>
+      </c>
+      <c r="N12" t="s">
+        <v>11</v>
+      </c>
+      <c r="O12" t="s">
+        <v>12</v>
+      </c>
+      <c r="P12" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>14</v>
+      </c>
+      <c r="R12" t="s">
+        <v>15</v>
+      </c>
+      <c r="S12" t="s">
+        <v>16</v>
+      </c>
+      <c r="T12" t="s">
+        <v>17</v>
+      </c>
+      <c r="U12" t="s">
+        <v>18</v>
+      </c>
+      <c r="V12" t="s">
+        <v>19</v>
+      </c>
+      <c r="W12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13">
+        <v>209</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K13" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13" t="s">
+        <v>10</v>
+      </c>
+      <c r="N13" t="s">
+        <v>11</v>
+      </c>
+      <c r="O13" t="s">
+        <v>12</v>
+      </c>
+      <c r="P13" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R13" t="s">
+        <v>15</v>
+      </c>
+      <c r="S13" t="s">
+        <v>16</v>
+      </c>
+      <c r="T13" t="s">
+        <v>17</v>
+      </c>
+      <c r="U13" t="s">
+        <v>18</v>
+      </c>
+      <c r="V13" t="s">
+        <v>19</v>
+      </c>
+      <c r="W13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14">
+        <v>211</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" t="s">
+        <v>10</v>
+      </c>
+      <c r="N14" t="s">
+        <v>11</v>
+      </c>
+      <c r="O14" t="s">
+        <v>12</v>
+      </c>
+      <c r="P14" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>14</v>
+      </c>
+      <c r="R14" t="s">
+        <v>15</v>
+      </c>
+      <c r="S14" t="s">
+        <v>16</v>
+      </c>
+      <c r="T14" t="s">
+        <v>17</v>
+      </c>
+      <c r="U14" t="s">
+        <v>18</v>
+      </c>
+      <c r="V14" t="s">
+        <v>19</v>
+      </c>
+      <c r="W14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15">
+        <v>211</v>
+      </c>
+      <c r="D15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J15" t="s">
+        <v>7</v>
+      </c>
+      <c r="K15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L15" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" t="s">
+        <v>10</v>
+      </c>
+      <c r="N15" t="s">
+        <v>11</v>
+      </c>
+      <c r="O15" t="s">
+        <v>12</v>
+      </c>
+      <c r="P15" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>14</v>
+      </c>
+      <c r="R15" t="s">
+        <v>15</v>
+      </c>
+      <c r="S15" t="s">
+        <v>16</v>
+      </c>
+      <c r="T15" t="s">
+        <v>17</v>
+      </c>
+      <c r="U15" t="s">
+        <v>18</v>
+      </c>
+      <c r="V15" t="s">
+        <v>19</v>
+      </c>
+      <c r="W15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16">
+        <v>211</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" t="s">
+        <v>8</v>
+      </c>
+      <c r="L16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N16" t="s">
+        <v>11</v>
+      </c>
+      <c r="O16" t="s">
+        <v>12</v>
+      </c>
+      <c r="P16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>14</v>
+      </c>
+      <c r="R16" t="s">
+        <v>15</v>
+      </c>
+      <c r="S16" t="s">
+        <v>16</v>
+      </c>
+      <c r="T16" t="s">
+        <v>17</v>
+      </c>
+      <c r="U16" t="s">
+        <v>18</v>
+      </c>
+      <c r="V16" t="s">
+        <v>19</v>
+      </c>
+      <c r="W16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
+      <c r="A17">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17">
+        <v>210</v>
+      </c>
+      <c r="D17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" t="s">
+        <v>8</v>
+      </c>
+      <c r="L17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" t="s">
+        <v>10</v>
+      </c>
+      <c r="N17" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17" t="s">
+        <v>12</v>
+      </c>
+      <c r="P17" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>14</v>
+      </c>
+      <c r="R17" t="s">
+        <v>15</v>
+      </c>
+      <c r="S17" t="s">
+        <v>16</v>
+      </c>
+      <c r="T17" t="s">
+        <v>17</v>
+      </c>
+      <c r="U17" t="s">
+        <v>18</v>
+      </c>
+      <c r="V17" t="s">
+        <v>19</v>
+      </c>
+      <c r="W17" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="19" spans="1:23">
       <c r="A19" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
         <v>67</v>
       </c>
       <c r="D19">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:23">
       <c r="A20">
-        <v>2</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="B20" s="2">
+        <v>5802.73</v>
       </c>
       <c r="C20">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="D20" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="F20" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="G20" t="s">
-        <v>4</v>
+        <v>73</v>
       </c>
       <c r="H20" t="s">
         <v>5</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>6</v>
+      <c r="I20" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="J20" t="s">
         <v>7</v>
@@ -677,31 +1588,31 @@
     </row>
     <row r="21" spans="1:23">
       <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>5692.87</v>
       </c>
       <c r="C21">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="D21" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="F21" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="G21" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="H21" t="s">
         <v>5</v>
       </c>
-      <c r="I21" t="s">
-        <v>26</v>
+      <c r="I21" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="J21" t="s">
         <v>7</v>
@@ -750,28 +1661,28 @@
       <c r="A22">
         <v>7</v>
       </c>
-      <c r="B22" t="s">
-        <v>27</v>
+      <c r="B22">
+        <v>5168.78</v>
       </c>
       <c r="C22">
-        <v>211</v>
+        <v>224</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="E22" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="F22" t="s">
-        <v>30</v>
+        <v>80</v>
       </c>
       <c r="G22" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="H22" t="s">
-        <v>5</v>
-      </c>
-      <c r="I22" t="s">
+        <v>142</v>
+      </c>
+      <c r="I22" s="4" t="s">
         <v>32</v>
       </c>
       <c r="J22" t="s">
@@ -819,31 +1730,31 @@
     </row>
     <row r="23" spans="1:23">
       <c r="A23">
-        <v>6</v>
-      </c>
-      <c r="B23" t="s">
-        <v>33</v>
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>4966.66</v>
       </c>
       <c r="C23">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="E23" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="F23" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="G23" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="H23" t="s">
         <v>5</v>
       </c>
-      <c r="I23" t="s">
-        <v>38</v>
+      <c r="I23" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="J23" t="s">
         <v>7</v>
@@ -890,31 +1801,31 @@
     </row>
     <row r="24" spans="1:23">
       <c r="A24">
-        <v>9</v>
-      </c>
-      <c r="B24" t="s">
-        <v>39</v>
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>4438.1499999999996</v>
       </c>
       <c r="C24">
-        <v>209</v>
+        <v>227</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="F24" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="G24" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="H24" t="s">
         <v>5</v>
       </c>
-      <c r="I24" t="s">
-        <v>43</v>
+      <c r="I24" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="J24" t="s">
         <v>7</v>
@@ -961,31 +1872,31 @@
     </row>
     <row r="25" spans="1:23">
       <c r="A25">
-        <v>4</v>
-      </c>
-      <c r="B25" t="s">
-        <v>44</v>
+        <v>2</v>
+      </c>
+      <c r="B25">
+        <v>3972.65</v>
       </c>
       <c r="C25">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="E25" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="F25" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="G25" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="H25" t="s">
         <v>5</v>
       </c>
-      <c r="I25" t="s">
-        <v>49</v>
+      <c r="I25" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="J25" t="s">
         <v>7</v>
@@ -1032,31 +1943,31 @@
     </row>
     <row r="26" spans="1:23">
       <c r="A26">
-        <v>3</v>
-      </c>
-      <c r="B26" t="s">
-        <v>50</v>
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>3557.85</v>
       </c>
       <c r="C26">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="E26" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="F26" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="G26" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="H26" t="s">
         <v>5</v>
       </c>
-      <c r="I26" t="s">
-        <v>54</v>
+      <c r="I26" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="J26" t="s">
         <v>7</v>
@@ -1101,145 +2012,724 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
-      <c r="A27">
-        <v>5</v>
-      </c>
-      <c r="B27" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27">
-        <v>211</v>
-      </c>
-      <c r="D27" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" t="s">
-        <v>57</v>
-      </c>
-      <c r="F27" t="s">
-        <v>58</v>
-      </c>
-      <c r="G27" t="s">
-        <v>59</v>
-      </c>
-      <c r="H27" t="s">
-        <v>5</v>
-      </c>
-      <c r="I27" t="s">
+    <row r="28" spans="1:23">
+      <c r="A28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23">
+      <c r="A29">
+        <v>7</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29">
+        <v>219</v>
+      </c>
+      <c r="D29" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G29" t="s">
+        <v>99</v>
+      </c>
+      <c r="H29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J29" t="s">
+        <v>7</v>
+      </c>
+      <c r="K29" t="s">
+        <v>8</v>
+      </c>
+      <c r="L29" t="s">
+        <v>9</v>
+      </c>
+      <c r="M29" t="s">
+        <v>10</v>
+      </c>
+      <c r="N29" t="s">
+        <v>11</v>
+      </c>
+      <c r="O29" t="s">
+        <v>12</v>
+      </c>
+      <c r="P29" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>14</v>
+      </c>
+      <c r="R29" t="s">
+        <v>15</v>
+      </c>
+      <c r="S29" t="s">
+        <v>16</v>
+      </c>
+      <c r="T29" t="s">
+        <v>17</v>
+      </c>
+      <c r="U29" t="s">
+        <v>18</v>
+      </c>
+      <c r="V29" t="s">
+        <v>19</v>
+      </c>
+      <c r="W29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23">
+      <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30">
+        <v>219</v>
+      </c>
+      <c r="D30" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" t="s">
+        <v>103</v>
+      </c>
+      <c r="H30" t="s">
+        <v>5</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J30" t="s">
+        <v>7</v>
+      </c>
+      <c r="K30" t="s">
+        <v>8</v>
+      </c>
+      <c r="L30" t="s">
+        <v>9</v>
+      </c>
+      <c r="M30" t="s">
+        <v>10</v>
+      </c>
+      <c r="N30" t="s">
+        <v>11</v>
+      </c>
+      <c r="O30" t="s">
+        <v>12</v>
+      </c>
+      <c r="P30" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>14</v>
+      </c>
+      <c r="R30" t="s">
+        <v>15</v>
+      </c>
+      <c r="S30" t="s">
+        <v>16</v>
+      </c>
+      <c r="T30" t="s">
+        <v>17</v>
+      </c>
+      <c r="U30" t="s">
+        <v>18</v>
+      </c>
+      <c r="V30" t="s">
+        <v>19</v>
+      </c>
+      <c r="W30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23">
+      <c r="A31">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31">
+        <v>218</v>
+      </c>
+      <c r="D31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" t="s">
+        <v>107</v>
+      </c>
+      <c r="G31" t="s">
+        <v>108</v>
+      </c>
+      <c r="H31" t="s">
+        <v>5</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="J31" t="s">
+        <v>7</v>
+      </c>
+      <c r="K31" t="s">
+        <v>8</v>
+      </c>
+      <c r="L31" t="s">
+        <v>9</v>
+      </c>
+      <c r="M31" t="s">
+        <v>10</v>
+      </c>
+      <c r="N31" t="s">
+        <v>11</v>
+      </c>
+      <c r="O31" t="s">
+        <v>12</v>
+      </c>
+      <c r="P31" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>14</v>
+      </c>
+      <c r="R31" t="s">
+        <v>15</v>
+      </c>
+      <c r="S31" t="s">
+        <v>16</v>
+      </c>
+      <c r="T31" t="s">
+        <v>17</v>
+      </c>
+      <c r="U31" t="s">
+        <v>18</v>
+      </c>
+      <c r="V31" t="s">
+        <v>19</v>
+      </c>
+      <c r="W31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23">
+      <c r="A32">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32">
+        <v>217</v>
+      </c>
+      <c r="D32" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" t="s">
+        <v>110</v>
+      </c>
+      <c r="F32" t="s">
+        <v>111</v>
+      </c>
+      <c r="G32" t="s">
+        <v>112</v>
+      </c>
+      <c r="H32" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J32" t="s">
+        <v>7</v>
+      </c>
+      <c r="K32" t="s">
+        <v>8</v>
+      </c>
+      <c r="L32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M32" t="s">
+        <v>10</v>
+      </c>
+      <c r="N32" t="s">
+        <v>11</v>
+      </c>
+      <c r="O32" t="s">
+        <v>12</v>
+      </c>
+      <c r="P32" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>14</v>
+      </c>
+      <c r="R32" t="s">
+        <v>15</v>
+      </c>
+      <c r="S32" t="s">
+        <v>16</v>
+      </c>
+      <c r="T32" t="s">
+        <v>17</v>
+      </c>
+      <c r="U32" t="s">
+        <v>18</v>
+      </c>
+      <c r="V32" t="s">
+        <v>19</v>
+      </c>
+      <c r="W32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23">
+      <c r="A33">
+        <v>9</v>
+      </c>
+      <c r="B33" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33">
+        <v>217</v>
+      </c>
+      <c r="D33" t="s">
+        <v>114</v>
+      </c>
+      <c r="E33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F33" t="s">
+        <v>116</v>
+      </c>
+      <c r="G33" t="s">
+        <v>117</v>
+      </c>
+      <c r="H33" t="s">
+        <v>5</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="J33" t="s">
+        <v>7</v>
+      </c>
+      <c r="K33" t="s">
+        <v>8</v>
+      </c>
+      <c r="L33" t="s">
+        <v>9</v>
+      </c>
+      <c r="M33" t="s">
+        <v>10</v>
+      </c>
+      <c r="N33" t="s">
+        <v>11</v>
+      </c>
+      <c r="O33" t="s">
+        <v>12</v>
+      </c>
+      <c r="P33" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>14</v>
+      </c>
+      <c r="R33" t="s">
+        <v>15</v>
+      </c>
+      <c r="S33" t="s">
+        <v>16</v>
+      </c>
+      <c r="T33" t="s">
+        <v>17</v>
+      </c>
+      <c r="U33" t="s">
+        <v>18</v>
+      </c>
+      <c r="V33" t="s">
+        <v>19</v>
+      </c>
+      <c r="W33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34">
+        <v>219</v>
+      </c>
+      <c r="D34" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" t="s">
+        <v>120</v>
+      </c>
+      <c r="F34" t="s">
+        <v>121</v>
+      </c>
+      <c r="G34" t="s">
+        <v>122</v>
+      </c>
+      <c r="H34" t="s">
+        <v>5</v>
+      </c>
+      <c r="I34" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="J27" t="s">
-        <v>7</v>
-      </c>
-      <c r="K27" t="s">
+      <c r="J34" t="s">
+        <v>7</v>
+      </c>
+      <c r="K34" t="s">
         <v>8</v>
       </c>
-      <c r="L27" t="s">
-        <v>9</v>
-      </c>
-      <c r="M27" t="s">
+      <c r="L34" t="s">
+        <v>9</v>
+      </c>
+      <c r="M34" t="s">
         <v>10</v>
       </c>
-      <c r="N27" t="s">
+      <c r="N34" t="s">
         <v>11</v>
       </c>
-      <c r="O27" t="s">
+      <c r="O34" t="s">
         <v>12</v>
       </c>
-      <c r="P27" t="s">
+      <c r="P34" t="s">
         <v>13</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="Q34" t="s">
         <v>14</v>
       </c>
-      <c r="R27" t="s">
+      <c r="R34" t="s">
         <v>15</v>
       </c>
-      <c r="S27" t="s">
+      <c r="S34" t="s">
         <v>16</v>
       </c>
-      <c r="T27" t="s">
+      <c r="T34" t="s">
         <v>17</v>
       </c>
-      <c r="U27" t="s">
+      <c r="U34" t="s">
         <v>18</v>
       </c>
-      <c r="V27" t="s">
+      <c r="V34" t="s">
         <v>19</v>
       </c>
-      <c r="W27" t="s">
+      <c r="W34" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
-      <c r="A28">
+    <row r="35" spans="1:23">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>123</v>
+      </c>
+      <c r="C35">
+        <v>220</v>
+      </c>
+      <c r="D35" t="s">
+        <v>124</v>
+      </c>
+      <c r="E35" t="s">
+        <v>125</v>
+      </c>
+      <c r="F35" t="s">
+        <v>126</v>
+      </c>
+      <c r="G35" t="s">
+        <v>127</v>
+      </c>
+      <c r="H35" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J35" t="s">
+        <v>7</v>
+      </c>
+      <c r="K35" t="s">
         <v>8</v>
       </c>
-      <c r="B28" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28">
-        <v>210</v>
-      </c>
-      <c r="D28" t="s">
-        <v>62</v>
-      </c>
-      <c r="E28" t="s">
-        <v>63</v>
-      </c>
-      <c r="F28" t="s">
-        <v>64</v>
-      </c>
-      <c r="G28" t="s">
-        <v>65</v>
-      </c>
-      <c r="H28" t="s">
-        <v>5</v>
-      </c>
-      <c r="I28" t="s">
-        <v>66</v>
-      </c>
-      <c r="J28" t="s">
-        <v>7</v>
-      </c>
-      <c r="K28" t="s">
+      <c r="L35" t="s">
+        <v>9</v>
+      </c>
+      <c r="M35" t="s">
+        <v>10</v>
+      </c>
+      <c r="N35" t="s">
+        <v>11</v>
+      </c>
+      <c r="O35" t="s">
+        <v>12</v>
+      </c>
+      <c r="P35" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>14</v>
+      </c>
+      <c r="R35" t="s">
+        <v>15</v>
+      </c>
+      <c r="S35" t="s">
+        <v>16</v>
+      </c>
+      <c r="T35" t="s">
+        <v>17</v>
+      </c>
+      <c r="U35" t="s">
+        <v>18</v>
+      </c>
+      <c r="V35" t="s">
+        <v>19</v>
+      </c>
+      <c r="W35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>128</v>
+      </c>
+      <c r="C36">
+        <v>219</v>
+      </c>
+      <c r="D36" t="s">
+        <v>124</v>
+      </c>
+      <c r="E36" t="s">
+        <v>129</v>
+      </c>
+      <c r="F36" t="s">
+        <v>130</v>
+      </c>
+      <c r="G36" t="s">
+        <v>131</v>
+      </c>
+      <c r="H36" t="s">
+        <v>5</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J36" t="s">
+        <v>7</v>
+      </c>
+      <c r="K36" t="s">
         <v>8</v>
       </c>
-      <c r="L28" t="s">
-        <v>9</v>
-      </c>
-      <c r="M28" t="s">
+      <c r="L36" t="s">
+        <v>9</v>
+      </c>
+      <c r="M36" t="s">
         <v>10</v>
       </c>
-      <c r="N28" t="s">
+      <c r="N36" t="s">
         <v>11</v>
       </c>
-      <c r="O28" t="s">
+      <c r="O36" t="s">
         <v>12</v>
       </c>
-      <c r="P28" t="s">
+      <c r="P36" t="s">
         <v>13</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="Q36" t="s">
         <v>14</v>
       </c>
-      <c r="R28" t="s">
+      <c r="R36" t="s">
         <v>15</v>
       </c>
-      <c r="S28" t="s">
+      <c r="S36" t="s">
         <v>16</v>
       </c>
-      <c r="T28" t="s">
+      <c r="T36" t="s">
         <v>17</v>
       </c>
-      <c r="U28" t="s">
+      <c r="U36" t="s">
         <v>18</v>
       </c>
-      <c r="V28" t="s">
+      <c r="V36" t="s">
         <v>19</v>
       </c>
-      <c r="W28" t="s">
+      <c r="W36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37">
+        <v>225</v>
+      </c>
+      <c r="D37" t="s">
+        <v>133</v>
+      </c>
+      <c r="E37" t="s">
+        <v>134</v>
+      </c>
+      <c r="F37" t="s">
+        <v>135</v>
+      </c>
+      <c r="G37" t="s">
+        <v>136</v>
+      </c>
+      <c r="H37" t="s">
+        <v>5</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J37" t="s">
+        <v>7</v>
+      </c>
+      <c r="K37" t="s">
+        <v>8</v>
+      </c>
+      <c r="L37" t="s">
+        <v>9</v>
+      </c>
+      <c r="M37" t="s">
+        <v>10</v>
+      </c>
+      <c r="N37" t="s">
+        <v>11</v>
+      </c>
+      <c r="O37" t="s">
+        <v>12</v>
+      </c>
+      <c r="P37" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>14</v>
+      </c>
+      <c r="R37" t="s">
+        <v>15</v>
+      </c>
+      <c r="S37" t="s">
+        <v>16</v>
+      </c>
+      <c r="T37" t="s">
+        <v>17</v>
+      </c>
+      <c r="U37" t="s">
+        <v>18</v>
+      </c>
+      <c r="V37" t="s">
+        <v>19</v>
+      </c>
+      <c r="W37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38">
+        <v>223</v>
+      </c>
+      <c r="D38" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" t="s">
+        <v>138</v>
+      </c>
+      <c r="F38" t="s">
+        <v>139</v>
+      </c>
+      <c r="G38" t="s">
+        <v>140</v>
+      </c>
+      <c r="H38" t="s">
+        <v>5</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J38" t="s">
+        <v>7</v>
+      </c>
+      <c r="K38" t="s">
+        <v>8</v>
+      </c>
+      <c r="L38" t="s">
+        <v>9</v>
+      </c>
+      <c r="M38" t="s">
+        <v>10</v>
+      </c>
+      <c r="N38" t="s">
+        <v>11</v>
+      </c>
+      <c r="O38" t="s">
+        <v>12</v>
+      </c>
+      <c r="P38" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>14</v>
+      </c>
+      <c r="R38" t="s">
+        <v>15</v>
+      </c>
+      <c r="S38" t="s">
+        <v>16</v>
+      </c>
+      <c r="T38" t="s">
+        <v>17</v>
+      </c>
+      <c r="U38" t="s">
+        <v>18</v>
+      </c>
+      <c r="V38" t="s">
+        <v>19</v>
+      </c>
+      <c r="W38" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>